<commit_message>
full functionality in vendors
</commit_message>
<xml_diff>
--- a/excel/Vendedores.xlsx
+++ b/excel/Vendedores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\VI\Bases de datos II\db_manager_xlcs_conv\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18950E0-A10B-453C-B679-48658AABAC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F9BA87-63B6-498D-923E-C60A1C6FE186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="97">
-  <si>
-    <t>ID Vendedor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="96">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -653,7 +650,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,14 +686,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -707,32 +701,29 @@
       <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
+      <c r="E2" s="2">
+        <v>5000</v>
       </c>
       <c r="F2" s="2">
-        <v>5000</v>
+        <v>4500</v>
       </c>
       <c r="G2" s="2">
-        <v>4500</v>
+        <v>300</v>
       </c>
       <c r="H2" s="2">
-        <v>300</v>
-      </c>
-      <c r="I2" s="2">
         <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -743,32 +734,29 @@
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2">
+        <v>4000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4200</v>
+      </c>
+      <c r="G3" s="2">
+        <v>250</v>
+      </c>
+      <c r="H3" s="2">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2">
-        <v>4000</v>
-      </c>
-      <c r="G3" s="2">
-        <v>4200</v>
-      </c>
-      <c r="H3" s="2">
-        <v>250</v>
-      </c>
-      <c r="I3" s="2">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -779,32 +767,29 @@
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="2">
+        <v>6000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5800</v>
+      </c>
+      <c r="G4" s="2">
+        <v>350</v>
+      </c>
+      <c r="H4" s="2">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2">
-        <v>6000</v>
-      </c>
-      <c r="G4" s="2">
-        <v>5800</v>
-      </c>
-      <c r="H4" s="2">
-        <v>350</v>
-      </c>
-      <c r="I4" s="2">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
@@ -815,32 +800,29 @@
       <c r="D5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="2">
+        <v>5500</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5600</v>
+      </c>
+      <c r="G5" s="2">
+        <v>400</v>
+      </c>
+      <c r="H5" s="2">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2">
-        <v>5500</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5600</v>
-      </c>
-      <c r="H5" s="2">
-        <v>400</v>
-      </c>
-      <c r="I5" s="2">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
@@ -851,566 +833,518 @@
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="2">
+        <v>7000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6900</v>
+      </c>
+      <c r="G6" s="2">
+        <v>500</v>
+      </c>
+      <c r="H6" s="2">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="2">
-        <v>7000</v>
-      </c>
-      <c r="G6" s="2">
-        <v>6900</v>
-      </c>
-      <c r="H6" s="2">
-        <v>500</v>
-      </c>
-      <c r="I6" s="2">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
       <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2800</v>
+      </c>
+      <c r="G7" s="2">
+        <v>150</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2">
-        <v>3000</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2800</v>
-      </c>
-      <c r="H7" s="2">
-        <v>150</v>
-      </c>
-      <c r="I7" s="2">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
       <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="2">
+        <v>4000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4300</v>
+      </c>
+      <c r="G8" s="2">
+        <v>300</v>
+      </c>
+      <c r="H8" s="2">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="2">
-        <v>4000</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4300</v>
-      </c>
-      <c r="H8" s="2">
-        <v>300</v>
-      </c>
-      <c r="I8" s="2">
-        <v>12</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
       <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="2">
+        <v>3500</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3700</v>
+      </c>
+      <c r="G9" s="2">
+        <v>200</v>
+      </c>
+      <c r="H9" s="2">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2">
-        <v>3500</v>
-      </c>
-      <c r="G9" s="2">
-        <v>3700</v>
-      </c>
-      <c r="H9" s="2">
-        <v>200</v>
-      </c>
-      <c r="I9" s="2">
-        <v>11</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
       <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>51</v>
+      <c r="E10" s="2">
+        <v>5000</v>
       </c>
       <c r="F10" s="2">
         <v>5000</v>
       </c>
       <c r="G10" s="2">
-        <v>5000</v>
+        <v>400</v>
       </c>
       <c r="H10" s="2">
-        <v>400</v>
-      </c>
-      <c r="I10" s="2">
         <v>13</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
       <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="2">
+        <v>4500</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4700</v>
+      </c>
+      <c r="G11" s="2">
+        <v>250</v>
+      </c>
+      <c r="H11" s="2">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="2">
-        <v>4500</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4700</v>
-      </c>
-      <c r="H11" s="2">
-        <v>250</v>
-      </c>
-      <c r="I11" s="2">
-        <v>16</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="2">
+        <v>2800</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2600</v>
+      </c>
+      <c r="G12" s="2">
+        <v>100</v>
+      </c>
+      <c r="H12" s="2">
+        <v>9</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="2">
-        <v>2800</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2600</v>
-      </c>
-      <c r="H12" s="2">
-        <v>100</v>
-      </c>
-      <c r="I12" s="2">
-        <v>9</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
       <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="2">
+        <v>3200</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3100</v>
+      </c>
+      <c r="G13" s="2">
+        <v>180</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="2">
-        <v>3200</v>
-      </c>
-      <c r="G13" s="2">
-        <v>3100</v>
-      </c>
-      <c r="H13" s="2">
-        <v>180</v>
-      </c>
-      <c r="I13" s="2">
-        <v>10</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
       <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="2">
+        <v>4000</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3900</v>
+      </c>
+      <c r="G14" s="2">
+        <v>240</v>
+      </c>
+      <c r="H14" s="2">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="2">
-        <v>4000</v>
-      </c>
-      <c r="G14" s="2">
-        <v>3900</v>
-      </c>
-      <c r="H14" s="2">
-        <v>240</v>
-      </c>
-      <c r="I14" s="2">
-        <v>12</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="2" t="s">
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
       <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="2">
+        <v>3500</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3400</v>
+      </c>
+      <c r="G15" s="2">
+        <v>220</v>
+      </c>
+      <c r="H15" s="2">
+        <v>11</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="2">
-        <v>3500</v>
-      </c>
-      <c r="G15" s="2">
-        <v>3400</v>
-      </c>
-      <c r="H15" s="2">
-        <v>220</v>
-      </c>
-      <c r="I15" s="2">
-        <v>11</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
       <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="2">
+        <v>6000</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5900</v>
+      </c>
+      <c r="G16" s="2">
+        <v>450</v>
+      </c>
+      <c r="H16" s="2">
+        <v>19</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="2">
-        <v>6000</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5900</v>
-      </c>
-      <c r="H16" s="2">
-        <v>450</v>
-      </c>
-      <c r="I16" s="2">
-        <v>19</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="2" t="s">
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
       <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="2">
+        <v>2700</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2600</v>
+      </c>
+      <c r="G17" s="2">
+        <v>120</v>
+      </c>
+      <c r="H17" s="2">
+        <v>8</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="2">
-        <v>2700</v>
-      </c>
-      <c r="G17" s="2">
-        <v>2600</v>
-      </c>
-      <c r="H17" s="2">
-        <v>120</v>
-      </c>
-      <c r="I17" s="2">
-        <v>8</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="2">
+        <v>4500</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4400</v>
+      </c>
+      <c r="G18" s="2">
+        <v>230</v>
+      </c>
+      <c r="H18" s="2">
+        <v>15</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F18" s="2">
-        <v>4500</v>
-      </c>
-      <c r="G18" s="2">
-        <v>4400</v>
-      </c>
-      <c r="H18" s="2">
-        <v>230</v>
-      </c>
-      <c r="I18" s="2">
-        <v>15</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="2" t="s">
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
       <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2900</v>
+      </c>
+      <c r="G19" s="2">
+        <v>170</v>
+      </c>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="2">
-        <v>3000</v>
-      </c>
-      <c r="G19" s="2">
-        <v>2900</v>
-      </c>
-      <c r="H19" s="2">
-        <v>170</v>
-      </c>
-      <c r="I19" s="2">
-        <v>10</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
       <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5200</v>
+      </c>
+      <c r="G20" s="2">
+        <v>350</v>
+      </c>
+      <c r="H20" s="2">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="2">
-        <v>5000</v>
-      </c>
-      <c r="G20" s="2">
-        <v>5200</v>
-      </c>
-      <c r="H20" s="2">
-        <v>350</v>
-      </c>
-      <c r="I20" s="2">
-        <v>14</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="2" t="s">
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
       <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="2">
+        <v>4000</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4100</v>
+      </c>
+      <c r="G21" s="2">
+        <v>260</v>
+      </c>
+      <c r="H21" s="2">
+        <v>12</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="F21" s="2">
-        <v>4000</v>
-      </c>
-      <c r="G21" s="2">
-        <v>4100</v>
-      </c>
-      <c r="H21" s="2">
-        <v>260</v>
-      </c>
-      <c r="I21" s="2">
-        <v>12</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="M21" s="3"/>
     </row>

</xml_diff>